<commit_message>
Include pharmacist assessment logic in model AB#15894
- Tidy up documentation for model properties
- Simplify logic populating medication summary
- Update front-end to use new model properties
- Update parameter names in medication report
- Update fixture and functional tests
</commit_message>
<xml_diff>
--- a/Apps/GatewayApi/src/Assets/Templates/MedicationReport.xlsx
+++ b/Apps/GatewayApi/src/Assets/Templates/MedicationReport.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_bugs\Apps\WebClient\src\Server\Assets\Templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646CA638-967C-4DAF-9B5E-2A0359CAED47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB37E560-E5F9-49BB-BFC9-AF50932BE6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
+    <workbookView xWindow="9630" yWindow="2730" windowWidth="25980" windowHeight="17190" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,9 +67,6 @@
     <t>{d.records[i].din_pin}</t>
   </si>
   <si>
-    <t>{d.records[i].generic}</t>
-  </si>
-  <si>
     <t>{d.records[i].practitioner}</t>
   </si>
   <si>
@@ -93,9 +85,6 @@
     <t>{d.records[i+1].din_pin}</t>
   </si>
   <si>
-    <t>{d.records[i+1].generic}</t>
-  </si>
-  <si>
     <t>{d.records[i+1].practitioner}</t>
   </si>
   <si>
@@ -111,10 +100,16 @@
     <t>{d.records[i+1].manufacturer}</t>
   </si>
   <si>
-    <t>{d.records[i].brand}</t>
-  </si>
-  <si>
-    <t>{d.records[i+1].brand}</t>
+    <t>{d.records[i].title}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].title}</t>
+  </si>
+  <si>
+    <t>{d.records[i].subtitle}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].subtitle}</t>
   </si>
 </sst>
 </file>
@@ -166,14 +161,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,21 +483,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60882D5E-E61D-5940-8D5B-09478E4A9588}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.296875" customWidth="1"/>
-    <col min="3" max="5" width="35.796875" customWidth="1"/>
+    <col min="1" max="1" width="14.25" customWidth="1"/>
+    <col min="3" max="5" width="35.75" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="30.796875" customWidth="1"/>
-    <col min="9" max="9" width="44.19921875" customWidth="1"/>
+    <col min="8" max="8" width="30.75" customWidth="1"/>
+    <col min="9" max="9" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -532,65 +523,66 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Include pharmacist assessment logic in model AB#15894 (#5608)
- Tidy up documentation for model properties
- Simplify logic populating medication summary
- Update front-end to use new model properties
- Update parameter names in medication report
- Update fixture and functional tests
</commit_message>
<xml_diff>
--- a/Apps/GatewayApi/src/Assets/Templates/MedicationReport.xlsx
+++ b/Apps/GatewayApi/src/Assets/Templates/MedicationReport.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_bugs\Apps\WebClient\src\Server\Assets\Templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646CA638-967C-4DAF-9B5E-2A0359CAED47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB37E560-E5F9-49BB-BFC9-AF50932BE6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
+    <workbookView xWindow="9630" yWindow="2730" windowWidth="25980" windowHeight="17190" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,9 +67,6 @@
     <t>{d.records[i].din_pin}</t>
   </si>
   <si>
-    <t>{d.records[i].generic}</t>
-  </si>
-  <si>
     <t>{d.records[i].practitioner}</t>
   </si>
   <si>
@@ -93,9 +85,6 @@
     <t>{d.records[i+1].din_pin}</t>
   </si>
   <si>
-    <t>{d.records[i+1].generic}</t>
-  </si>
-  <si>
     <t>{d.records[i+1].practitioner}</t>
   </si>
   <si>
@@ -111,10 +100,16 @@
     <t>{d.records[i+1].manufacturer}</t>
   </si>
   <si>
-    <t>{d.records[i].brand}</t>
-  </si>
-  <si>
-    <t>{d.records[i+1].brand}</t>
+    <t>{d.records[i].title}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].title}</t>
+  </si>
+  <si>
+    <t>{d.records[i].subtitle}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].subtitle}</t>
   </si>
 </sst>
 </file>
@@ -166,14 +161,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,21 +483,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60882D5E-E61D-5940-8D5B-09478E4A9588}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.296875" customWidth="1"/>
-    <col min="3" max="5" width="35.796875" customWidth="1"/>
+    <col min="1" max="1" width="14.25" customWidth="1"/>
+    <col min="3" max="5" width="35.75" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="30.796875" customWidth="1"/>
-    <col min="9" max="9" width="44.19921875" customWidth="1"/>
+    <col min="8" max="8" width="30.75" customWidth="1"/>
+    <col min="9" max="9" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -532,65 +523,66 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>